<commit_message>
add vertex 42 imagery to copyright sheet
</commit_message>
<xml_diff>
--- a/ReferenceFiles/Templates/assemblyOrderTemplate.xlsx
+++ b/ReferenceFiles/Templates/assemblyOrderTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15140" yWindow="0" windowWidth="13660" windowHeight="16480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="15140" yWindow="0" windowWidth="13660" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="©" sheetId="2" r:id="rId1"/>
@@ -722,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B16"/>
+  <dimension ref="B1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -739,50 +739,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
-      <c r="B3" t="s">
+    <row r="3" spans="2:2" ht="37" customHeight="1"/>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="2:2">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="2:2">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="30">
-      <c r="B8" s="9" t="s">
+    <row r="9" spans="2:2" ht="30">
+      <c r="B9" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="30">
-      <c r="B10" s="9" t="s">
+    <row r="11" spans="2:2" ht="30">
+      <c r="B11" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="30">
-      <c r="B12" s="9" t="s">
+    <row r="13" spans="2:2" ht="30">
+      <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
-      <c r="B14" s="1" t="s">
+    <row r="15" spans="2:2">
+      <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:2">
-      <c r="B16" s="2" t="s">
+    <row r="17" spans="2:2">
+      <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B15" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -797,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
fuss with default print settings
</commit_message>
<xml_diff>
--- a/ReferenceFiles/Templates/assemblyOrderTemplate.xlsx
+++ b/ReferenceFiles/Templates/assemblyOrderTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5060" yWindow="0" windowWidth="24260" windowHeight="17240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1680" yWindow="1680" windowWidth="23920" windowHeight="14380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="©" sheetId="2" r:id="rId1"/>
@@ -358,32 +358,32 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -811,13 +811,13 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
     <col min="3" max="3" width="6.83203125" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" customWidth="1"/>
@@ -826,8 +826,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="49" customHeight="1">
-      <c r="A1" s="25"/>
-      <c r="B1" s="25"/>
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="20" t="s">
         <v>9</v>
       </c>
@@ -837,27 +837,27 @@
       <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="29" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
       <c r="D2" s="18"/>
-      <c r="E2" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="26"/>
+      <c r="E2" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="25"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1">
-      <c r="A3" s="21"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="26"/>
+      <c r="E3" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="25"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="20">
@@ -867,10 +867,10 @@
       <c r="B4" s="32"/>
       <c r="C4" s="32"/>
       <c r="D4" s="19"/>
-      <c r="E4" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="26"/>
+      <c r="E4" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="25"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="7" customHeight="1">
@@ -883,19 +883,19 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="19" customHeight="1">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="29"/>
+      <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1">
       <c r="A7" s="8"/>
@@ -1210,15 +1210,15 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
modify to handle time estimates
</commit_message>
<xml_diff>
--- a/ReferenceFiles/Templates/assemblyOrderTemplate.xlsx
+++ b/ReferenceFiles/Templates/assemblyOrderTemplate.xlsx
@@ -110,14 +110,6 @@
       <color indexed="12"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -164,7 +156,14 @@
       <name val="Trebuchet MS"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -314,14 +313,14 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -338,28 +337,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -368,32 +367,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -811,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1211,19 +1210,20 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="31"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="32"/>
       <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="A33:C33"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="C6:E6"/>
-    <mergeCell ref="A33:G33"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
@@ -1234,7 +1234,7 @@
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="B4:C4"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
reformat to include zacks needs
</commit_message>
<xml_diff>
--- a/ReferenceFiles/Templates/assemblyOrderTemplate.xlsx
+++ b/ReferenceFiles/Templates/assemblyOrderTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Packing Slip Template</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Product:</t>
   </si>
   <si>
-    <t>Date Completed:</t>
-  </si>
-  <si>
     <t>Assembler:</t>
   </si>
   <si>
@@ -70,17 +67,23 @@
     <t>Order Quantity</t>
   </si>
   <si>
-    <t>Date Started:</t>
-  </si>
-  <si>
     <t>Quantity:</t>
+  </si>
+  <si>
+    <t>Date of Assembly:</t>
+  </si>
+  <si>
+    <t>Time Completed:</t>
+  </si>
+  <si>
+    <t>Time Started:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,12 +126,6 @@
       <name val="Trebuchet MS"/>
     </font>
     <font>
-      <b/>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -166,8 +163,30 @@
       <sz val="12"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +199,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -245,17 +270,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -307,56 +321,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -364,9 +378,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -376,26 +387,47 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -404,6 +436,15 @@
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -747,7 +788,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="21">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -768,17 +809,17 @@
       </c>
     </row>
     <row r="9" spans="2:2" ht="30">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="30">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="30">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -808,433 +849,422 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:C33"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="6.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="49" customHeight="1">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="20" t="s">
+    <row r="1" spans="1:10" ht="49" customHeight="1">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" ht="20" customHeight="1">
-      <c r="A2" s="27" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:10" ht="20" customHeight="1">
+      <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="23" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="1:10" ht="20">
+      <c r="A3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:10" ht="16" customHeight="1">
+      <c r="A4" s="23"/>
+      <c r="B4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="24"/>
+    </row>
+    <row r="5" spans="1:10" ht="16" customHeight="1">
+      <c r="A5" s="23"/>
+      <c r="B5" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="24"/>
+    </row>
+    <row r="6" spans="1:10" ht="7" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="19" customHeight="1">
+      <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="20" customHeight="1">
-      <c r="A3" s="27"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="20">
-      <c r="A4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="7" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="19" customHeight="1">
-      <c r="A6" s="24" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="21" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="1:7" ht="19" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10" t="str">
-        <f>IF($D7="","",$D7*$B$4)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="19" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13" t="str">
-        <f t="shared" ref="G8:G32" si="0">IF($D8="","",$D8*$B$4)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="19" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="19" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="19" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="19" customHeight="1">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="19" customHeight="1">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="19" customHeight="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="19" customHeight="1">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="19" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="19" customHeight="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="19" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="19" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="19" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="19" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="19" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="19" customHeight="1">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="19" customHeight="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="19" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="19" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="19" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="19" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="19" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="19" customHeight="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="19" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="19" customHeight="1">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="32"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:10" ht="19" customHeight="1">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7" t="str">
+        <f>IF($D8="","",$D8*$B$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="19" customHeight="1">
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9" t="str">
+        <f t="shared" ref="F9:F32" si="0">IF($D9="","",$D9*$B$3)</f>
+        <v/>
+      </c>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:10" ht="19" customHeight="1">
+      <c r="A10" s="30"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="19" customHeight="1">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="19" customHeight="1">
+      <c r="A12" s="30"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="19" customHeight="1">
+      <c r="A13" s="30"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="19" customHeight="1">
+      <c r="A14" s="30"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="19" customHeight="1">
+      <c r="A15" s="30"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="19" customHeight="1">
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="19" customHeight="1">
+      <c r="A17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="19" customHeight="1">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="19" customHeight="1">
+      <c r="A19" s="30"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="19" customHeight="1">
+      <c r="A20" s="30"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="19" customHeight="1">
+      <c r="A21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="19" customHeight="1">
+      <c r="A22" s="30"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="19" customHeight="1">
+      <c r="A23" s="30"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="19" customHeight="1">
+      <c r="A24" s="30"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="19" customHeight="1">
+      <c r="A25" s="30"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="19" customHeight="1">
+      <c r="A26" s="30"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="19" customHeight="1">
+      <c r="A27" s="30"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="19" customHeight="1">
+      <c r="A28" s="30"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="19" customHeight="1">
+      <c r="A29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="19" customHeight="1">
+      <c r="A30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="19" customHeight="1">
+      <c r="A31" s="30"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="19" customHeight="1">
+      <c r="A32" s="30"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="D33:G33"/>
+  <mergeCells count="36">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D33:F33"/>
     <mergeCell ref="A33:C33"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
custom sort and other small fixes
</commit_message>
<xml_diff>
--- a/ReferenceFiles/Templates/assemblyOrderTemplate.xlsx
+++ b/ReferenceFiles/Templates/assemblyOrderTemplate.xlsx
@@ -366,6 +366,30 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -387,44 +411,20 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -866,58 +866,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="49" customHeight="1">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="33" t="s">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="32"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="20" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="20">
       <c r="A3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:10" ht="16" customHeight="1">
-      <c r="A4" s="23"/>
-      <c r="B4" s="26" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="24"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:10" ht="16" customHeight="1">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="24"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="7" customHeight="1">
       <c r="A6" s="3"/>
@@ -928,22 +928,22 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16" t="s">
+      <c r="D7" s="24"/>
+      <c r="E7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1">
-      <c r="A8" s="28"/>
-      <c r="B8" s="29"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -953,8 +953,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -962,11 +962,11 @@
         <f t="shared" ref="F9:F32" si="0">IF($D9="","",$D9*$B$3)</f>
         <v/>
       </c>
-      <c r="J9" s="27"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -976,8 +976,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1">
-      <c r="A11" s="30"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -987,8 +987,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="19" customHeight="1">
-      <c r="A12" s="30"/>
-      <c r="B12" s="31"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -998,8 +998,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="19" customHeight="1">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1009,8 +1009,8 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="19" customHeight="1">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1020,8 +1020,8 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1031,8 +1031,8 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="19" customHeight="1">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -1042,8 +1042,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="19" customHeight="1">
-      <c r="A17" s="30"/>
-      <c r="B17" s="31"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -1053,8 +1053,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="19" customHeight="1">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -1064,8 +1064,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="19" customHeight="1">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1075,8 +1075,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="19" customHeight="1">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -1086,8 +1086,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="19" customHeight="1">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -1097,8 +1097,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="19" customHeight="1">
-      <c r="A22" s="30"/>
-      <c r="B22" s="31"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -1108,8 +1108,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="19" customHeight="1">
-      <c r="A23" s="30"/>
-      <c r="B23" s="31"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -1119,8 +1119,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="19" customHeight="1">
-      <c r="A24" s="30"/>
-      <c r="B24" s="31"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -1130,8 +1130,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="19" customHeight="1">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="33"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -1141,8 +1141,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="19" customHeight="1">
-      <c r="A26" s="30"/>
-      <c r="B26" s="31"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="33"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1152,8 +1152,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="19" customHeight="1">
-      <c r="A27" s="30"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -1163,8 +1163,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="19" customHeight="1">
-      <c r="A28" s="30"/>
-      <c r="B28" s="31"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -1174,8 +1174,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="19" customHeight="1">
-      <c r="A29" s="30"/>
-      <c r="B29" s="31"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -1185,8 +1185,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="19" customHeight="1">
-      <c r="A30" s="30"/>
-      <c r="B30" s="31"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
@@ -1196,8 +1196,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="19" customHeight="1">
-      <c r="A31" s="30"/>
-      <c r="B31" s="31"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -1207,8 +1207,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="19" customHeight="1">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="33"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -1218,51 +1218,51 @@
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>